<commit_message>
Verifying proper updating. Stopped at slide 36.
Took 4 hours 21 minutes

Took 2 minutes
</commit_message>
<xml_diff>
--- a/src/AE_LIW_automation/output/AE_LIW_Excel_output.xlsx
+++ b/src/AE_LIW_automation/output/AE_LIW_Excel_output.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15960" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="36920" yWindow="3020" windowWidth="28800" windowHeight="15960" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -16,7 +16,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="2">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -28,6 +28,13 @@
       <name val="Calibri"/>
       <family val="2"/>
       <sz val="8"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -51,17 +58,20 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="5">
+  <dxfs count="6">
     <dxf>
       <numFmt numFmtId="13" formatCode="0%"/>
     </dxf>
@@ -73,6 +83,9 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" wrapText="1"/>
     </dxf>
     <dxf>
       <alignment horizontal="general" vertical="bottom" wrapText="1"/>
@@ -151,16 +164,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1343" displayName="Table1343" ref="A1:E7" headerRowCount="1" totalsRowShown="0" headerRowDxfId="4">
-  <sortState ref="A2:D9">
-    <sortCondition descending="1" ref="D2:D9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1343" displayName="Table1343" ref="A1:E8" headerRowCount="1" totalsRowShown="0" headerRowDxfId="5">
+  <sortState ref="A2:B9">
+    <sortCondition descending="1" ref="B2:B9"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" name=" "/>
-    <tableColumn id="16" name="Q4 2023_x000a_(N=28)" dataDxfId="3"/>
-    <tableColumn id="17" name="Q1 2024_x000a_(N=12)" dataDxfId="2"/>
-    <tableColumn id="19" name="Q2 2024_x000a_(N=44)" dataDxfId="1"/>
-    <tableColumn id="18" name="Q3 2024_x000a_(N=19)" dataDxfId="0"/>
+    <tableColumn id="1" name=" " dataDxfId="4"/>
+    <tableColumn id="19" name="Q3 2024_x000a_(N=19)" dataDxfId="3"/>
+    <tableColumn id="18" name="Q4 2024_x000a_(N=33)" dataDxfId="2"/>
+    <tableColumn id="2" name="Q1 2025_x000a_(N=45)" dataDxfId="1"/>
+    <tableColumn id="3" name="Q2 2025_x000a_(N=46)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -433,15 +446,16 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:L9"/>
+  <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="87" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
     <col width="25" customWidth="1" min="1" max="1"/>
+    <col width="19.83203125" bestFit="1" customWidth="1" min="7" max="7"/>
   </cols>
   <sheetData>
     <row r="1" ht="63" customHeight="1">
@@ -452,259 +466,190 @@
       </c>
       <c r="B1" s="2" t="inlineStr">
         <is>
-          <t>Q4 2023
-(N=28)</t>
-        </is>
-      </c>
-      <c r="C1" s="2" t="inlineStr">
-        <is>
-          <t>Q1 2024
-(N=12)</t>
-        </is>
-      </c>
-      <c r="D1" s="2" t="inlineStr">
-        <is>
-          <t>Q2 2024
-(N=44)</t>
-        </is>
-      </c>
-      <c r="E1" s="2" t="inlineStr">
-        <is>
           <t>Q3 2024
 (N=19)</t>
         </is>
       </c>
-      <c r="H1" t="inlineStr">
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>Q4 2024
+(N=33)</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
+        <is>
+          <t>Q1 2025
+(N=45)</t>
+        </is>
+      </c>
+      <c r="E1" s="3" t="inlineStr">
+        <is>
+          <t>Q2 2025
+(N=46)</t>
+        </is>
+      </c>
+      <c r="F1" s="3" t="n"/>
+      <c r="H1" s="1" t="n"/>
+      <c r="I1" s="1" t="n"/>
+      <c r="J1" s="1" t="n"/>
+    </row>
+    <row r="2" ht="16" customHeight="1">
+      <c r="A2" s="2" t="inlineStr">
         <is>
           <t xml:space="preserve">Email </t>
         </is>
       </c>
-      <c r="I1" s="1" t="n">
-        <v>0.73</v>
-      </c>
-      <c r="J1" s="1" t="n">
-        <v>0.63</v>
-      </c>
-      <c r="K1" s="1" t="n">
-        <v>0.73</v>
-      </c>
-      <c r="L1" s="1" t="n">
-        <v>0.63</v>
-      </c>
-    </row>
-    <row r="2" ht="63" customHeight="1">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Email </t>
-        </is>
-      </c>
       <c r="B2" s="1" t="n">
-        <v>0.43</v>
+        <v>0.631578947368421</v>
       </c>
       <c r="C2" s="1" t="n">
-        <v>0.75</v>
+        <v>0.7575757575757576</v>
       </c>
       <c r="D2" s="1" t="n">
-        <v>0.7045454545454546</v>
+        <v>0.71</v>
       </c>
       <c r="E2" s="1" t="n">
-        <v>0.631578947368421</v>
-      </c>
-      <c r="H2" t="inlineStr">
+        <v>0.59</v>
+      </c>
+      <c r="F2" s="1" t="n"/>
+      <c r="H2" s="1" t="n"/>
+      <c r="I2" s="1" t="n"/>
+      <c r="J2" s="1" t="n"/>
+    </row>
+    <row r="3" ht="16" customHeight="1">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>Text messages</t>
+        </is>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>0.2105263157894737</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>0.4545454545454545</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>0.38</v>
+      </c>
+      <c r="E3" s="1" t="n">
+        <v>0.3</v>
+      </c>
+      <c r="F3" s="1" t="n"/>
+      <c r="H3" s="1" t="n"/>
+      <c r="I3" s="1" t="n"/>
+      <c r="J3" s="1" t="n"/>
+    </row>
+    <row r="4" ht="16" customHeight="1">
+      <c r="A4" s="2" t="inlineStr">
         <is>
           <t>Phone call</t>
         </is>
       </c>
-      <c r="I2" s="1" t="n">
+      <c r="B4" s="1" t="n">
+        <v>0.3157894736842105</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>0.2424242424242424</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="E4" s="1" t="n">
         <v>0.15</v>
       </c>
-      <c r="J2" s="1" t="n">
-        <v>0.31</v>
-      </c>
-      <c r="K2" s="1" t="n">
-        <v>0.28</v>
-      </c>
-      <c r="L2" s="1" t="n">
-        <v>0.5600000000000001</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>Phone call</t>
-        </is>
-      </c>
-      <c r="B3" s="1" t="n">
-        <v>0.29</v>
-      </c>
-      <c r="C3" s="1" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="D3" s="1" t="n">
-        <v>0.1590909090909091</v>
-      </c>
-      <c r="E3" s="1" t="n">
-        <v>0.3157894736842105</v>
-      </c>
-      <c r="H3" t="inlineStr">
-        <is>
-          <t>Text messages</t>
-        </is>
-      </c>
-      <c r="I3" s="1" t="n">
-        <v>0.08</v>
-      </c>
-      <c r="J3" s="1" t="n">
-        <v>0.06</v>
-      </c>
-      <c r="K3" s="1" t="n">
-        <v>0.23</v>
-      </c>
-      <c r="L3" s="1" t="n">
-        <v>0.38</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="inlineStr">
-        <is>
-          <t>Text messages</t>
-        </is>
-      </c>
-      <c r="B4" s="1" t="n">
-        <v>0.21</v>
-      </c>
-      <c r="C4" s="1" t="n">
-        <v>0.17</v>
-      </c>
-      <c r="D4" s="1" t="n">
-        <v>0.1363636363636364</v>
-      </c>
-      <c r="E4" s="1" t="n">
-        <v>0.2105263157894737</v>
-      </c>
-      <c r="H4" t="inlineStr">
+      <c r="F4" s="1" t="n"/>
+      <c r="H4" s="1" t="n"/>
+      <c r="I4" s="1" t="n"/>
+      <c r="J4" s="1" t="n"/>
+    </row>
+    <row r="5" ht="16" customHeight="1">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>Austin Energy's Website</t>
+        </is>
+      </c>
+      <c r="B5" s="1" t="n"/>
+      <c r="C5" s="1" t="n">
+        <v>0.1212121212121212</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <v>0.22</v>
+      </c>
+      <c r="F5" s="1" t="n"/>
+      <c r="H5" s="1" t="n"/>
+      <c r="I5" s="1" t="n"/>
+      <c r="J5" s="1" t="n"/>
+    </row>
+    <row r="6" ht="16" customHeight="1">
+      <c r="A6" s="2" t="inlineStr">
         <is>
           <t>Direct mail</t>
         </is>
       </c>
-      <c r="I4" s="1" t="n">
-        <v>0.23</v>
-      </c>
-      <c r="J4" s="1" t="n">
-        <v>0.25</v>
-      </c>
-      <c r="K4" s="1" t="n">
-        <v>0.33</v>
-      </c>
-      <c r="L4" s="1" t="n">
-        <v>0.31</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="inlineStr">
-        <is>
-          <t>Direct mail</t>
-        </is>
-      </c>
-      <c r="B5" s="1" t="n">
-        <v>0.18</v>
-      </c>
-      <c r="C5" s="1" t="n"/>
-      <c r="D5" s="1" t="n">
-        <v>0.1136363636363636</v>
-      </c>
-      <c r="E5" s="1" t="n">
+      <c r="B6" s="1" t="n">
         <v>0.1052631578947368</v>
       </c>
-      <c r="H5" t="inlineStr">
-        <is>
-          <t>Austin Energy's Website</t>
-        </is>
-      </c>
-      <c r="I5" s="1" t="n">
+      <c r="C6" s="1" t="n">
+        <v>0.09090909090909093</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>0.44</v>
+      </c>
+      <c r="E6" s="1" t="n">
+        <v>0.41</v>
+      </c>
+      <c r="F6" s="1" t="n"/>
+      <c r="G6" s="2" t="n"/>
+      <c r="H6" s="1" t="n"/>
+      <c r="I6" s="1" t="n"/>
+      <c r="J6" s="1" t="n"/>
+    </row>
+    <row r="7" ht="32" customHeight="1">
+      <c r="A7" s="2" t="inlineStr">
+        <is>
+          <t>Facebook, Twitter, or other Social Media</t>
+        </is>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v>0.0303030303030303</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="E7" s="1" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="F7" s="1" t="n"/>
+      <c r="H7" s="1" t="n"/>
+      <c r="I7" s="1" t="n"/>
+      <c r="J7" s="1" t="n"/>
+    </row>
+    <row r="8" ht="16" customHeight="1">
+      <c r="A8" s="2" t="inlineStr">
+        <is>
+          <t>All other</t>
+        </is>
+      </c>
+      <c r="B8" s="1" t="n">
+        <v>0.05263157894736842</v>
+      </c>
+      <c r="C8" s="1" t="n">
+        <v>0.05263157894736842</v>
+      </c>
+      <c r="D8" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="J5" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="K5" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L5" s="1" t="n">
-        <v>0.06</v>
-      </c>
-    </row>
-    <row r="6" ht="96" customHeight="1">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>Austin Energy's Website</t>
-        </is>
-      </c>
-      <c r="B6" s="1" t="n">
-        <v>0.04</v>
-      </c>
-      <c r="C6" s="1" t="n"/>
-      <c r="E6" s="1" t="n"/>
-      <c r="H6" s="2" t="inlineStr">
-        <is>
-          <t>Facebook, Twitter, or 
-other Social media</t>
-        </is>
-      </c>
-      <c r="I6" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="J6" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="K6" s="1" t="n">
-        <v>0.23</v>
-      </c>
-      <c r="L6" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7">
-      <c r="A7" t="inlineStr">
-        <is>
-          <t>All other</t>
-        </is>
-      </c>
-      <c r="B7" s="1" t="n"/>
-      <c r="C7" s="1" t="n"/>
-      <c r="D7" s="1" t="n">
-        <v>0.02272727272727273</v>
-      </c>
-      <c r="E7" s="1" t="n">
-        <v>0.05263157894736842</v>
-      </c>
-      <c r="H7" t="inlineStr">
-        <is>
-          <t>Door hangers</t>
-        </is>
-      </c>
-      <c r="I7" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="J7" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="K7" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="L7" s="1" t="n">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8">
-      <c r="D8" s="1" t="n"/>
-      <c r="E8" s="1" t="n"/>
+      <c r="E8" s="1" t="n">
+        <v>0.14</v>
+      </c>
+      <c r="F8" s="1" t="n"/>
     </row>
     <row r="9">
       <c r="B9" s="1" t="n"/>
       <c r="C9" s="1" t="n"/>
-      <c r="D9" s="1" t="n"/>
-      <c r="E9" s="1" t="n"/>
     </row>
     <row r="10"/>
     <row r="11"/>

</xml_diff>

<commit_message>
slide_43_py refactor using get_data_blob_from_chart() WIP.
Took 1 hour 19 minutes
</commit_message>
<xml_diff>
--- a/src/AE_LIW_automation/output/AE_LIW_Excel_output.xlsx
+++ b/src/AE_LIW_automation/output/AE_LIW_Excel_output.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="36920" yWindow="3020" windowWidth="28800" windowHeight="15960" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="1440" yWindow="760" windowWidth="28800" windowHeight="15960" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -16,7 +16,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="5">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -27,7 +27,21 @@
     <font>
       <name val="Calibri"/>
       <family val="2"/>
-      <sz val="8"/>
+      <color theme="1"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Arial"/>
+      <family val="2"/>
+      <color rgb="FF264A60"/>
+      <sz val="12"/>
+    </font>
+    <font>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <color rgb="FF000000"/>
+      <sz val="12"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -38,15 +52,21 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE0E0E0"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -54,41 +74,74 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color rgb="FFAEAEAE"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFAEAEAE"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="9">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment wrapText="1"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="9" fontId="2" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="9">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="1" builtinId="5"/>
+    <cellStyle name="style1686767965002" xfId="2"/>
+    <cellStyle name="style1686767965016" xfId="3"/>
+    <cellStyle name="style1686767965169" xfId="4"/>
+    <cellStyle name="style1686767964769" xfId="5"/>
+    <cellStyle name="style1686767965192" xfId="6"/>
+    <cellStyle name="style1686767965204" xfId="7"/>
+    <cellStyle name="style1706365766073" xfId="8"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="1">
     <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="13" formatCode="0%"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" wrapText="1"/>
-    </dxf>
-    <dxf>
-      <alignment horizontal="general" vertical="bottom" wrapText="1"/>
+      <font>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <strike val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <condense val="0"/>
+        <color rgb="FF000000"/>
+        <extend val="0"/>
+        <sz val="12"/>
+        <vertAlign val="baseline"/>
+        <scheme val="minor"/>
+      </font>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -164,16 +217,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1343" displayName="Table1343" ref="A1:E8" headerRowCount="1" totalsRowShown="0" headerRowDxfId="5">
-  <sortState ref="A2:B9">
-    <sortCondition descending="1" ref="B2:B9"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table122213" displayName="Table122213" ref="A1:E12" headerRowCount="1" totalsRowShown="0">
+  <sortState ref="A2:E11">
+    <sortCondition ref="D2:D12"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" name=" " dataDxfId="4"/>
-    <tableColumn id="19" name="Q3 2024_x000a_(N=19)" dataDxfId="3"/>
-    <tableColumn id="18" name="Q4 2024_x000a_(N=33)" dataDxfId="2"/>
-    <tableColumn id="2" name="Q1 2025_x000a_(N=45)" dataDxfId="1"/>
-    <tableColumn id="3" name="Q2 2025_x000a_(N=46)" dataDxfId="0"/>
+    <tableColumn id="1" name=" "/>
+    <tableColumn id="3" name="Q1 2025_x000a_(N=45)" dataDxfId="0" dataCellStyle="Percent"/>
+    <tableColumn id="19" name="Q4 2024_x000a_(N=33)"/>
+    <tableColumn id="18" name="Q3 2024_x000a_(N=19)"/>
+    <tableColumn id="17" name="Q2 2024_x000a_(N=44)"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -446,214 +499,221 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J9"/>
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="87" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col width="25" customWidth="1" min="1" max="1"/>
-    <col width="19.83203125" bestFit="1" customWidth="1" min="7" max="7"/>
+    <col width="22.83203125" bestFit="1" customWidth="1" min="1" max="1"/>
+    <col width="8" bestFit="1" customWidth="1" min="2" max="2"/>
+    <col width="7.6640625" bestFit="1" customWidth="1" min="3" max="5"/>
   </cols>
   <sheetData>
-    <row r="1" ht="63" customHeight="1">
-      <c r="A1" t="inlineStr">
+    <row r="1" ht="51" customHeight="1">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>Q1 2025
+(N=45)</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>Q4 2024
+(N=33)</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>Q3 2024
 (N=19)</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
-        <is>
-          <t>Q4 2024
-(N=33)</t>
-        </is>
-      </c>
-      <c r="D1" s="2" t="inlineStr">
-        <is>
-          <t>Q1 2025
-(N=45)</t>
-        </is>
-      </c>
-      <c r="E1" s="3" t="inlineStr">
-        <is>
-          <t>Q2 2025
-(N=46)</t>
-        </is>
-      </c>
-      <c r="F1" s="3" t="n"/>
-      <c r="H1" s="1" t="n"/>
-      <c r="I1" s="1" t="n"/>
-      <c r="J1" s="1" t="n"/>
+      <c r="E1" s="2" t="inlineStr">
+        <is>
+          <t>Q2 2024
+(N=44)</t>
+        </is>
+      </c>
     </row>
     <row r="2" ht="16" customHeight="1">
-      <c r="A2" s="2" t="inlineStr">
-        <is>
-          <t xml:space="preserve">Email </t>
-        </is>
-      </c>
-      <c r="B2" s="1" t="n">
-        <v>0.631578947368421</v>
-      </c>
-      <c r="C2" s="1" t="n">
-        <v>0.7575757575757576</v>
-      </c>
-      <c r="D2" s="1" t="n">
-        <v>0.71</v>
-      </c>
-      <c r="E2" s="1" t="n">
-        <v>0.59</v>
-      </c>
-      <c r="F2" s="1" t="n"/>
-      <c r="H2" s="1" t="n"/>
-      <c r="I2" s="1" t="n"/>
-      <c r="J2" s="1" t="n"/>
+      <c r="A2" s="1" t="inlineStr">
+        <is>
+          <t>All other</t>
+        </is>
+      </c>
+      <c r="B2" s="9" t="n"/>
+      <c r="C2" s="3" t="n"/>
+      <c r="D2" s="3" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="E2" s="3" t="n">
+        <v>0.11</v>
+      </c>
     </row>
     <row r="3" ht="16" customHeight="1">
-      <c r="A3" s="2" t="inlineStr">
-        <is>
-          <t>Text messages</t>
-        </is>
-      </c>
-      <c r="B3" s="1" t="n">
-        <v>0.2105263157894737</v>
-      </c>
-      <c r="C3" s="1" t="n">
-        <v>0.4545454545454545</v>
-      </c>
-      <c r="D3" s="1" t="n">
-        <v>0.38</v>
-      </c>
-      <c r="E3" s="1" t="n">
-        <v>0.3</v>
-      </c>
-      <c r="F3" s="1" t="n"/>
-      <c r="H3" s="1" t="n"/>
-      <c r="I3" s="1" t="n"/>
-      <c r="J3" s="1" t="n"/>
-    </row>
-    <row r="4" ht="16" customHeight="1">
-      <c r="A4" s="2" t="inlineStr">
-        <is>
-          <t>Phone call</t>
-        </is>
-      </c>
-      <c r="B4" s="1" t="n">
-        <v>0.3157894736842105</v>
-      </c>
-      <c r="C4" s="1" t="n">
-        <v>0.2424242424242424</v>
-      </c>
-      <c r="D4" s="1" t="n">
+      <c r="A3" s="1" t="inlineStr">
+        <is>
+          <t>Do not know</t>
+        </is>
+      </c>
+      <c r="B3" s="9" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="C3" s="3" t="n"/>
+      <c r="D3" s="3" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="E3" s="3" t="n">
         <v>0.07000000000000001</v>
       </c>
-      <c r="E4" s="1" t="n">
-        <v>0.15</v>
-      </c>
-      <c r="F4" s="1" t="n"/>
-      <c r="H4" s="1" t="n"/>
-      <c r="I4" s="1" t="n"/>
-      <c r="J4" s="1" t="n"/>
+    </row>
+    <row r="4" ht="17" customHeight="1">
+      <c r="A4" s="4" t="inlineStr">
+        <is>
+          <t>Austin 311</t>
+        </is>
+      </c>
+      <c r="B4" s="8" t="n"/>
+      <c r="C4" s="3" t="n"/>
+      <c r="D4" s="3" t="n"/>
+      <c r="E4" s="3" t="n"/>
     </row>
     <row r="5" ht="16" customHeight="1">
-      <c r="A5" s="2" t="inlineStr">
-        <is>
-          <t>Austin Energy's Website</t>
-        </is>
-      </c>
-      <c r="B5" s="1" t="n"/>
-      <c r="C5" s="1" t="n">
-        <v>0.1212121212121212</v>
-      </c>
-      <c r="D5" s="1" t="n">
-        <v>0.36</v>
-      </c>
-      <c r="E5" s="1" t="n">
-        <v>0.22</v>
-      </c>
-      <c r="F5" s="1" t="n"/>
-      <c r="H5" s="1" t="n"/>
-      <c r="I5" s="1" t="n"/>
-      <c r="J5" s="1" t="n"/>
+      <c r="A5" s="1" t="inlineStr">
+        <is>
+          <t>Austin Energy called me</t>
+        </is>
+      </c>
+      <c r="B5" s="9" t="n"/>
+      <c r="C5" s="3" t="n"/>
+      <c r="D5" s="3" t="n"/>
+      <c r="E5" s="3" t="n">
+        <v>0.02</v>
+      </c>
     </row>
     <row r="6" ht="16" customHeight="1">
-      <c r="A6" s="2" t="inlineStr">
-        <is>
-          <t>Direct mail</t>
-        </is>
-      </c>
-      <c r="B6" s="1" t="n">
-        <v>0.1052631578947368</v>
-      </c>
-      <c r="C6" s="1" t="n">
-        <v>0.09090909090909093</v>
-      </c>
-      <c r="D6" s="1" t="n">
-        <v>0.44</v>
-      </c>
-      <c r="E6" s="1" t="n">
-        <v>0.41</v>
-      </c>
-      <c r="F6" s="1" t="n"/>
-      <c r="G6" s="2" t="n"/>
-      <c r="H6" s="1" t="n"/>
-      <c r="I6" s="1" t="n"/>
-      <c r="J6" s="1" t="n"/>
-    </row>
-    <row r="7" ht="32" customHeight="1">
-      <c r="A7" s="2" t="inlineStr">
-        <is>
-          <t>Facebook, Twitter, or other Social Media</t>
-        </is>
-      </c>
-      <c r="C7" s="1" t="n">
-        <v>0.0303030303030303</v>
-      </c>
-      <c r="D7" s="1" t="n">
+      <c r="A6" s="1" t="inlineStr">
+        <is>
+          <t>On City's website</t>
+        </is>
+      </c>
+      <c r="B6" s="9" t="n">
         <v>0.09</v>
       </c>
-      <c r="E7" s="1" t="n">
-        <v>0.07000000000000001</v>
-      </c>
-      <c r="F7" s="1" t="n"/>
-      <c r="H7" s="1" t="n"/>
-      <c r="I7" s="1" t="n"/>
-      <c r="J7" s="1" t="n"/>
+      <c r="C6" s="3" t="n"/>
+      <c r="D6" s="3" t="n"/>
+      <c r="E6" s="3" t="n">
+        <v>0.09</v>
+      </c>
+    </row>
+    <row r="7" ht="16" customHeight="1">
+      <c r="A7" s="1" t="inlineStr">
+        <is>
+          <t>Utility bill insert/mail</t>
+        </is>
+      </c>
+      <c r="B7" s="9" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="C7" s="3" t="n"/>
+      <c r="D7" s="3" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="E7" s="3" t="n"/>
     </row>
     <row r="8" ht="16" customHeight="1">
-      <c r="A8" s="2" t="inlineStr">
-        <is>
-          <t>All other</t>
-        </is>
-      </c>
-      <c r="B8" s="1" t="n">
-        <v>0.05263157894736842</v>
-      </c>
-      <c r="C8" s="1" t="n">
-        <v>0.05263157894736842</v>
-      </c>
-      <c r="D8" s="1" t="n">
-        <v>0</v>
-      </c>
-      <c r="E8" s="1" t="n">
-        <v>0.14</v>
-      </c>
-      <c r="F8" s="1" t="n"/>
-    </row>
-    <row r="9">
-      <c r="B9" s="1" t="n"/>
-      <c r="C9" s="1" t="n"/>
-    </row>
-    <row r="10"/>
-    <row r="11"/>
-    <row r="12"/>
+      <c r="A8" s="1" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="B8" s="9" t="n">
+        <v>0.02</v>
+      </c>
+      <c r="C8" s="3" t="n"/>
+      <c r="D8" s="3" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="E8" s="5" t="n"/>
+    </row>
+    <row r="9" ht="16" customHeight="1">
+      <c r="A9" s="1" t="inlineStr">
+        <is>
+          <t>I called them</t>
+        </is>
+      </c>
+      <c r="B9" s="9" t="n"/>
+      <c r="C9" s="3" t="n">
+        <v>0.06</v>
+      </c>
+      <c r="D9" s="3" t="n">
+        <v>0.05</v>
+      </c>
+      <c r="E9" s="3" t="n">
+        <v>0.02</v>
+      </c>
+    </row>
+    <row r="10" ht="16" customHeight="1">
+      <c r="A10" s="1" t="inlineStr">
+        <is>
+          <t>Word of mouth</t>
+        </is>
+      </c>
+      <c r="B10" s="9" t="n">
+        <v>0.16</v>
+      </c>
+      <c r="C10" s="3" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="D10" s="3" t="n">
+        <v>0.11</v>
+      </c>
+      <c r="E10" s="3" t="n"/>
+    </row>
+    <row r="11" ht="16" customHeight="1">
+      <c r="A11" s="10" t="inlineStr">
+        <is>
+          <t>Utility Contact Center</t>
+        </is>
+      </c>
+      <c r="B11" s="9" t="n">
+        <v>0.04</v>
+      </c>
+      <c r="C11" s="3" t="n">
+        <v>0.18</v>
+      </c>
+      <c r="D11" s="3" t="n"/>
+      <c r="E11" s="3" t="n">
+        <v>0.18</v>
+      </c>
+    </row>
+    <row r="12" ht="16" customHeight="1">
+      <c r="A12" s="6" t="inlineStr">
+        <is>
+          <t>Austin Energy's website</t>
+        </is>
+      </c>
+      <c r="B12" s="9" t="n">
+        <v>0.53</v>
+      </c>
+      <c r="C12" s="3" t="n">
+        <v>0.67</v>
+      </c>
+      <c r="D12" s="3" t="n">
+        <v>0.58</v>
+      </c>
+      <c r="E12" s="3" t="n">
+        <v>0.5</v>
+      </c>
+    </row>
     <row r="13"/>
     <row r="14"/>
     <row r="15"/>
@@ -673,27 +733,6 @@
     <row r="29"/>
     <row r="30"/>
     <row r="31"/>
-    <row r="32"/>
-    <row r="33"/>
-    <row r="34"/>
-    <row r="35"/>
-    <row r="36"/>
-    <row r="37"/>
-    <row r="38"/>
-    <row r="39"/>
-    <row r="40"/>
-    <row r="41"/>
-    <row r="42"/>
-    <row r="43"/>
-    <row r="44"/>
-    <row r="45"/>
-    <row r="46"/>
-    <row r="47"/>
-    <row r="48"/>
-    <row r="49"/>
-    <row r="50"/>
-    <row r="51"/>
-    <row r="52"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
Verifying slide updaters function correctly. slide_45.py updates correctly and is last updater verified.
Took 1 hour 27 minutes
</commit_message>
<xml_diff>
--- a/src/AE_LIW_automation/output/AE_LIW_Excel_output.xlsx
+++ b/src/AE_LIW_automation/output/AE_LIW_Excel_output.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="1440" yWindow="760" windowWidth="28800" windowHeight="15960" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="17280" yWindow="760" windowWidth="17280" windowHeight="10800" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
@@ -16,7 +16,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="5">
+  <fonts count="3">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -27,21 +27,7 @@
     <font>
       <name val="Calibri"/>
       <family val="2"/>
-      <color theme="1"/>
-      <sz val="11"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Arial"/>
-      <family val="2"/>
-      <color rgb="FF264A60"/>
-      <sz val="12"/>
-    </font>
-    <font>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <color rgb="FF000000"/>
-      <sz val="12"/>
+      <sz val="8"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -52,21 +38,15 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="2">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFE0E0E0"/>
-        <bgColor rgb="FF000000"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="2">
+  <borders count="1">
     <border>
       <left/>
       <right/>
@@ -74,74 +54,41 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color rgb="FFAEAEAE"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFAEAEAE"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
-  <cellStyleXfs count="9">
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf numFmtId="9" fontId="2" fillId="2" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="9">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Percent" xfId="1" builtinId="5"/>
-    <cellStyle name="style1686767965002" xfId="2"/>
-    <cellStyle name="style1686767965016" xfId="3"/>
-    <cellStyle name="style1686767965169" xfId="4"/>
-    <cellStyle name="style1686767964769" xfId="5"/>
-    <cellStyle name="style1686767965192" xfId="6"/>
-    <cellStyle name="style1686767965204" xfId="7"/>
-    <cellStyle name="style1706365766073" xfId="8"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="6">
     <dxf>
-      <font>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <strike val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <condense val="0"/>
-        <color rgb="FF000000"/>
-        <extend val="0"/>
-        <sz val="12"/>
-        <vertAlign val="baseline"/>
-        <scheme val="minor"/>
-      </font>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="13" formatCode="0%"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" wrapText="1"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" wrapText="1"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -217,16 +164,16 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table122213" displayName="Table122213" ref="A1:E12" headerRowCount="1" totalsRowShown="0">
-  <sortState ref="A2:E11">
-    <sortCondition ref="D2:D12"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1343" displayName="Table1343" ref="A1:E8" headerRowCount="1" totalsRowShown="0" headerRowDxfId="5">
+  <sortState ref="A2:B9">
+    <sortCondition descending="1" ref="B2:B9"/>
   </sortState>
   <tableColumns count="5">
-    <tableColumn id="1" name=" "/>
-    <tableColumn id="3" name="Q1 2025_x000a_(N=45)" dataDxfId="0" dataCellStyle="Percent"/>
-    <tableColumn id="19" name="Q4 2024_x000a_(N=33)"/>
-    <tableColumn id="18" name="Q3 2024_x000a_(N=19)"/>
-    <tableColumn id="17" name="Q2 2024_x000a_(N=44)"/>
+    <tableColumn id="1" name=" " dataDxfId="4"/>
+    <tableColumn id="19" name="Q3 2024_x000a_(N=19)" dataDxfId="3"/>
+    <tableColumn id="18" name="Q4 2024_x000a_(N=33)" dataDxfId="2"/>
+    <tableColumn id="2" name="Q1 2025_x000a_(N=45)" dataDxfId="1"/>
+    <tableColumn id="3" name="Q2 2025_x000a_(N=46)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -499,221 +446,180 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="87" workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15"/>
   <cols>
-    <col width="22.83203125" bestFit="1" customWidth="1" min="1" max="1"/>
-    <col width="8" bestFit="1" customWidth="1" min="2" max="2"/>
-    <col width="7.6640625" bestFit="1" customWidth="1" min="3" max="5"/>
+    <col width="25" customWidth="1" min="1" max="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="51" customHeight="1">
-      <c r="A1" s="1" t="inlineStr">
+    <row r="1" ht="63" customHeight="1">
+      <c r="A1" t="inlineStr">
         <is>
           <t xml:space="preserve"> </t>
         </is>
       </c>
       <c r="B1" s="2" t="inlineStr">
+        <is>
+          <t>Q3 2024
+(N=19)</t>
+        </is>
+      </c>
+      <c r="C1" s="2" t="inlineStr">
+        <is>
+          <t>Q4 2024
+(N=33)</t>
+        </is>
+      </c>
+      <c r="D1" s="2" t="inlineStr">
         <is>
           <t>Q1 2025
 (N=45)</t>
         </is>
       </c>
-      <c r="C1" s="2" t="inlineStr">
-        <is>
-          <t>Q4 2024
-(N=33)</t>
-        </is>
-      </c>
-      <c r="D1" s="2" t="inlineStr">
-        <is>
-          <t>Q3 2024
-(N=19)</t>
-        </is>
-      </c>
-      <c r="E1" s="2" t="inlineStr">
-        <is>
-          <t>Q2 2024
-(N=44)</t>
+      <c r="E1" s="3" t="inlineStr">
+        <is>
+          <t>Q2 2025
+(N=46)</t>
         </is>
       </c>
     </row>
     <row r="2" ht="16" customHeight="1">
-      <c r="A2" s="1" t="inlineStr">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>Email</t>
+        </is>
+      </c>
+      <c r="B2" s="1" t="n">
+        <v>0.631578947368421</v>
+      </c>
+      <c r="C2" s="1" t="n">
+        <v>0.7575757575757576</v>
+      </c>
+      <c r="D2" s="1" t="n">
+        <v>0.71</v>
+      </c>
+      <c r="E2" s="1" t="n">
+        <v>0.59</v>
+      </c>
+    </row>
+    <row r="3" ht="16" customHeight="1">
+      <c r="A3" s="2" t="inlineStr">
+        <is>
+          <t>Text messages</t>
+        </is>
+      </c>
+      <c r="B3" s="1" t="n">
+        <v>0.2105263157894737</v>
+      </c>
+      <c r="C3" s="1" t="n">
+        <v>0.4545454545454545</v>
+      </c>
+      <c r="D3" s="1" t="n">
+        <v>0.38</v>
+      </c>
+      <c r="E3" s="1" t="n">
+        <v>0.3</v>
+      </c>
+    </row>
+    <row r="4" ht="16" customHeight="1">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>Phone call</t>
+        </is>
+      </c>
+      <c r="B4" s="1" t="n">
+        <v>0.3157894736842105</v>
+      </c>
+      <c r="C4" s="1" t="n">
+        <v>0.2424242424242424</v>
+      </c>
+      <c r="D4" s="1" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+      <c r="E4" s="1" t="n">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="5" ht="16" customHeight="1">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>Austin Energy's website</t>
+        </is>
+      </c>
+      <c r="B5" s="1" t="n"/>
+      <c r="C5" s="1" t="n">
+        <v>0.1212121212121212</v>
+      </c>
+      <c r="D5" s="1" t="n">
+        <v>0.36</v>
+      </c>
+      <c r="E5" s="1" t="n">
+        <v>0.22</v>
+      </c>
+    </row>
+    <row r="6" ht="16" customHeight="1">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>Direct mail</t>
+        </is>
+      </c>
+      <c r="B6" s="1" t="n">
+        <v>0.1052631578947368</v>
+      </c>
+      <c r="C6" s="1" t="n">
+        <v>0.09090909090909093</v>
+      </c>
+      <c r="D6" s="1" t="n">
+        <v>0.44</v>
+      </c>
+      <c r="E6" s="1" t="n">
+        <v>0.41</v>
+      </c>
+    </row>
+    <row r="7" ht="32" customHeight="1">
+      <c r="A7" s="2" t="inlineStr">
+        <is>
+          <t>Facebook, Twitter, or other Social Media</t>
+        </is>
+      </c>
+      <c r="C7" s="1" t="n">
+        <v>0.0303030303030303</v>
+      </c>
+      <c r="D7" s="1" t="n">
+        <v>0.09</v>
+      </c>
+      <c r="E7" s="1" t="n">
+        <v>0.07000000000000001</v>
+      </c>
+    </row>
+    <row r="8" ht="16" customHeight="1">
+      <c r="A8" s="2" t="inlineStr">
         <is>
           <t>All other</t>
         </is>
       </c>
-      <c r="B2" s="9" t="n"/>
-      <c r="C2" s="3" t="n"/>
-      <c r="D2" s="3" t="n">
-        <v>0.11</v>
-      </c>
-      <c r="E2" s="3" t="n">
-        <v>0.11</v>
-      </c>
-    </row>
-    <row r="3" ht="16" customHeight="1">
-      <c r="A3" s="1" t="inlineStr">
-        <is>
-          <t>Do not know</t>
-        </is>
-      </c>
-      <c r="B3" s="9" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="C3" s="3" t="n"/>
-      <c r="D3" s="3" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="E3" s="3" t="n">
-        <v>0.07000000000000001</v>
-      </c>
-    </row>
-    <row r="4" ht="17" customHeight="1">
-      <c r="A4" s="4" t="inlineStr">
-        <is>
-          <t>Austin 311</t>
-        </is>
-      </c>
-      <c r="B4" s="8" t="n"/>
-      <c r="C4" s="3" t="n"/>
-      <c r="D4" s="3" t="n"/>
-      <c r="E4" s="3" t="n"/>
-    </row>
-    <row r="5" ht="16" customHeight="1">
-      <c r="A5" s="1" t="inlineStr">
-        <is>
-          <t>Austin Energy called me</t>
-        </is>
-      </c>
-      <c r="B5" s="9" t="n"/>
-      <c r="C5" s="3" t="n"/>
-      <c r="D5" s="3" t="n"/>
-      <c r="E5" s="3" t="n">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="6" ht="16" customHeight="1">
-      <c r="A6" s="1" t="inlineStr">
-        <is>
-          <t>On City's website</t>
-        </is>
-      </c>
-      <c r="B6" s="9" t="n">
-        <v>0.09</v>
-      </c>
-      <c r="C6" s="3" t="n"/>
-      <c r="D6" s="3" t="n"/>
-      <c r="E6" s="3" t="n">
-        <v>0.09</v>
-      </c>
-    </row>
-    <row r="7" ht="16" customHeight="1">
-      <c r="A7" s="1" t="inlineStr">
-        <is>
-          <t>Utility bill insert/mail</t>
-        </is>
-      </c>
-      <c r="B7" s="9" t="n">
-        <v>0.04</v>
-      </c>
-      <c r="C7" s="3" t="n"/>
-      <c r="D7" s="3" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="E7" s="3" t="n"/>
-    </row>
-    <row r="8" ht="16" customHeight="1">
-      <c r="A8" s="1" t="inlineStr">
-        <is>
-          <t>Email</t>
-        </is>
-      </c>
-      <c r="B8" s="9" t="n">
-        <v>0.02</v>
-      </c>
-      <c r="C8" s="3" t="n"/>
-      <c r="D8" s="3" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="E8" s="5" t="n"/>
-    </row>
-    <row r="9" ht="16" customHeight="1">
-      <c r="A9" s="1" t="inlineStr">
-        <is>
-          <t>I called them</t>
-        </is>
-      </c>
-      <c r="B9" s="9" t="n"/>
-      <c r="C9" s="3" t="n">
-        <v>0.06</v>
-      </c>
-      <c r="D9" s="3" t="n">
-        <v>0.05</v>
-      </c>
-      <c r="E9" s="3" t="n">
-        <v>0.02</v>
-      </c>
-    </row>
-    <row r="10" ht="16" customHeight="1">
-      <c r="A10" s="1" t="inlineStr">
-        <is>
-          <t>Word of mouth</t>
-        </is>
-      </c>
-      <c r="B10" s="9" t="n">
-        <v>0.16</v>
-      </c>
-      <c r="C10" s="3" t="n">
-        <v>0.09</v>
-      </c>
-      <c r="D10" s="3" t="n">
-        <v>0.11</v>
-      </c>
-      <c r="E10" s="3" t="n"/>
-    </row>
-    <row r="11" ht="16" customHeight="1">
-      <c r="A11" s="10" t="inlineStr">
-        <is>
-          <t>Utility Contact Center</t>
-        </is>
-      </c>
-      <c r="B11" s="9" t="n">
-        <v>0.04</v>
-      </c>
-      <c r="C11" s="3" t="n">
-        <v>0.18</v>
-      </c>
-      <c r="D11" s="3" t="n"/>
-      <c r="E11" s="3" t="n">
-        <v>0.18</v>
-      </c>
-    </row>
-    <row r="12" ht="16" customHeight="1">
-      <c r="A12" s="6" t="inlineStr">
-        <is>
-          <t>Austin Energy's website</t>
-        </is>
-      </c>
-      <c r="B12" s="9" t="n">
-        <v>0.53</v>
-      </c>
-      <c r="C12" s="3" t="n">
-        <v>0.67</v>
-      </c>
-      <c r="D12" s="3" t="n">
-        <v>0.58</v>
-      </c>
-      <c r="E12" s="3" t="n">
-        <v>0.5</v>
-      </c>
-    </row>
+      <c r="B8" s="1" t="n">
+        <v>0.05263157894736842</v>
+      </c>
+      <c r="C8" s="1" t="n">
+        <v>0.05263157894736842</v>
+      </c>
+      <c r="D8" s="1" t="n">
+        <v>0</v>
+      </c>
+      <c r="E8" s="1" t="n">
+        <v>0.14</v>
+      </c>
+    </row>
+    <row r="9"/>
+    <row r="10"/>
+    <row r="11"/>
+    <row r="12"/>
     <row r="13"/>
     <row r="14"/>
     <row r="15"/>
@@ -733,6 +639,27 @@
     <row r="29"/>
     <row r="30"/>
     <row r="31"/>
+    <row r="32"/>
+    <row r="33"/>
+    <row r="34"/>
+    <row r="35"/>
+    <row r="36"/>
+    <row r="37"/>
+    <row r="38"/>
+    <row r="39"/>
+    <row r="40"/>
+    <row r="41"/>
+    <row r="42"/>
+    <row r="43"/>
+    <row r="44"/>
+    <row r="45"/>
+    <row r="46"/>
+    <row r="47"/>
+    <row r="48"/>
+    <row r="49"/>
+    <row r="50"/>
+    <row r="51"/>
+    <row r="52"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait"/>

</xml_diff>

<commit_message>
Consolidating 24Q1 through 25Q3 data into 25Q3 report.
Took 1 hour 0 minutes
</commit_message>
<xml_diff>
--- a/src/AE_LIW_automation/output/AE_LIW_Excel_output.xlsx
+++ b/src/AE_LIW_automation/output/AE_LIW_Excel_output.xlsx
@@ -429,28 +429,28 @@
     <row r="1">
       <c r="B1" t="inlineStr">
         <is>
-          <t>Q2 2024
-(N=44)</t>
-        </is>
-      </c>
-      <c r="C1" t="inlineStr">
-        <is>
           <t>Q3 2024
 (N=19)</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="C1" t="inlineStr">
         <is>
           <t>Q4 2024
 (N=33)</t>
         </is>
       </c>
-      <c r="E1" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>Q1 2025
 (N=45)</t>
         </is>
       </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Q2 2025
+(N=46)</t>
+        </is>
+      </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
@@ -465,10 +465,10 @@
         <v>0</v>
       </c>
       <c r="D2" s="3" t="n">
-        <v>0</v>
+        <v>0.7111111111111111</v>
       </c>
       <c r="E2" s="3" t="n">
-        <v>0.7111111111111111</v>
+        <v>0.5869565217391305</v>
       </c>
     </row>
     <row r="3">
@@ -478,16 +478,16 @@
         </is>
       </c>
       <c r="B3" s="3" t="n">
-        <v>0.1136363636363636</v>
+        <v>0.1052631578947368</v>
       </c>
       <c r="C3" s="3" t="n">
-        <v>0.1052631578947368</v>
+        <v>0.09090909090909093</v>
       </c>
       <c r="D3" s="3" t="n">
-        <v>0.09090909090909093</v>
+        <v>0.4444444444444444</v>
       </c>
       <c r="E3" s="3" t="n">
-        <v>0.4444444444444444</v>
+        <v>0.4130434782608696</v>
       </c>
     </row>
     <row r="4">
@@ -497,16 +497,16 @@
         </is>
       </c>
       <c r="B4" s="3" t="n">
-        <v>0.1363636363636364</v>
+        <v>0.2105263157894737</v>
       </c>
       <c r="C4" s="3" t="n">
-        <v>0.2105263157894737</v>
+        <v>0.4545454545454545</v>
       </c>
       <c r="D4" s="3" t="n">
-        <v>0.4545454545454545</v>
+        <v>0.3777777777777778</v>
       </c>
       <c r="E4" s="3" t="n">
-        <v>0.3777777777777778</v>
+        <v>0.3043478260869565</v>
       </c>
     </row>
     <row r="5">
@@ -522,16 +522,16 @@
         <v>0</v>
       </c>
       <c r="D5" s="3" t="n">
-        <v>0</v>
+        <v>0.3555555555555556</v>
       </c>
       <c r="E5" s="3" t="n">
-        <v>0.3555555555555556</v>
+        <v>0.2173913043478261</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Door hangers</t>
+          <t>Phone</t>
         </is>
       </c>
       <c r="B6" s="3" t="n">
@@ -541,16 +541,16 @@
         <v>0</v>
       </c>
       <c r="D6" s="3" t="n">
-        <v>0</v>
+        <v>0.06666666666666667</v>
       </c>
       <c r="E6" s="3" t="n">
-        <v>0.1333333333333333</v>
+        <v>0.1521739130434783</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Facebook, Twitter, or other Social Media</t>
+          <t>Door hangers</t>
         </is>
       </c>
       <c r="B7" s="3" t="n">
@@ -560,29 +560,29 @@
         <v>0</v>
       </c>
       <c r="D7" s="3" t="n">
-        <v>0.0303030303030303</v>
+        <v>0.1333333333333333</v>
       </c>
       <c r="E7" s="3" t="n">
-        <v>0.08888888888888889</v>
+        <v>0.06521739130434782</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Phone</t>
+          <t>Facebook, Twitter, or other Social Media</t>
         </is>
       </c>
       <c r="B8" s="3" t="n">
         <v>0</v>
       </c>
       <c r="C8" s="3" t="n">
-        <v>0</v>
+        <v>0.0303030303030303</v>
       </c>
       <c r="D8" s="3" t="n">
-        <v>0</v>
+        <v>0.08888888888888889</v>
       </c>
       <c r="E8" s="3" t="n">
-        <v>0.06666666666666667</v>
+        <v>0.06521739130434782</v>
       </c>
     </row>
     <row r="9">
@@ -592,13 +592,13 @@
         </is>
       </c>
       <c r="B9" s="3" t="n">
-        <v>0.7045454545454546</v>
+        <v>0.631578947368421</v>
       </c>
       <c r="C9" s="3" t="n">
-        <v>0.631578947368421</v>
+        <v>0.7575757575757576</v>
       </c>
       <c r="D9" s="3" t="n">
-        <v>0.7575757575757576</v>
+        <v>0</v>
       </c>
       <c r="E9" s="3" t="n">
         <v>0</v>
@@ -611,13 +611,13 @@
         </is>
       </c>
       <c r="B10" s="3" t="n">
-        <v>0.1590909090909091</v>
+        <v>0.3157894736842105</v>
       </c>
       <c r="C10" s="3" t="n">
-        <v>0.3157894736842105</v>
+        <v>0.2424242424242424</v>
       </c>
       <c r="D10" s="3" t="n">
-        <v>0.2424242424242424</v>
+        <v>0</v>
       </c>
       <c r="E10" s="3" t="n">
         <v>0</v>
@@ -633,10 +633,10 @@
         <v>0</v>
       </c>
       <c r="C11" s="3" t="n">
-        <v>0</v>
+        <v>0.1212121212121212</v>
       </c>
       <c r="D11" s="3" t="n">
-        <v>0.1212121212121212</v>
+        <v>0</v>
       </c>
       <c r="E11" s="3" t="n">
         <v>0</v>
@@ -649,16 +649,16 @@
         </is>
       </c>
       <c r="B12" s="3" t="n">
-        <v>0.02272727272727273</v>
+        <v>0.05263157894736842</v>
       </c>
       <c r="C12" s="3" t="n">
         <v>0.05263157894736842</v>
       </c>
       <c r="D12" s="3" t="n">
-        <v>0.05263157894736842</v>
+        <v>0</v>
       </c>
       <c r="E12" s="3" t="n">
-        <v>0</v>
+        <v>0.06521739130434782</v>
       </c>
     </row>
   </sheetData>

</xml_diff>